<commit_message>
Atualização de TOKEN JWT
</commit_message>
<xml_diff>
--- a/planilhas-comparacoes/relatoriosdwg_rev2_vs_rev4.xlsx
+++ b/planilhas-comparacoes/relatoriosdwg_rev2_vs_rev4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
   <si>
     <t xml:space="preserve">LISTA </t>
   </si>
@@ -242,6 +242,12 @@
     <t>ADICIONADO</t>
   </si>
   <si>
+    <t>10027489</t>
+  </si>
+  <si>
+    <t>tê para tubo</t>
+  </si>
+  <si>
     <t>10038562</t>
   </si>
   <si>
@@ -263,6 +269,9 @@
     <t>junta circular para flange</t>
   </si>
   <si>
+    <t>10334519</t>
+  </si>
+  <si>
     <t>10360352</t>
   </si>
   <si>
@@ -275,10 +284,10 @@
     <t>tubo condução de aço carbono</t>
   </si>
   <si>
-    <t>10390585</t>
+    <t>10390629</t>
   </si>
   <si>
-    <t>10390629</t>
+    <t>10515625</t>
   </si>
   <si>
     <t>10559349</t>
@@ -291,6 +300,9 @@
   </si>
   <si>
     <t>11389614</t>
+  </si>
+  <si>
+    <t>11399557</t>
   </si>
   <si>
     <t xml:space="preserve"> NOTAS:</t>
@@ -48754,7 +48766,7 @@
       <c r="AZ11" s="239"/>
       <c r="BA11" s="240"/>
       <c r="BB11" s="226">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BC11" s="227"/>
       <c r="BD11" s="227"/>
@@ -48762,7 +48774,7 @@
       <c r="BF11" s="227"/>
       <c r="BG11" s="228"/>
       <c r="BH11" s="226">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="BI11" s="227"/>
       <c r="BJ11" s="227"/>
@@ -49262,7 +49274,7 @@
       <c r="AT17" s="246"/>
       <c r="AU17" s="246"/>
       <c r="AV17" s="247">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW17" s="247"/>
       <c r="AX17" s="247"/>
@@ -49278,14 +49290,14 @@
       <c r="BF17" s="233"/>
       <c r="BG17" s="233"/>
       <c r="BH17" s="226">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BI17" s="227"/>
       <c r="BJ17" s="227"/>
       <c r="BK17" s="227"/>
       <c r="BL17" s="228"/>
       <c r="BM17" s="226" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="BN17" s="227"/>
       <c r="BO17" s="227"/>
@@ -49348,7 +49360,7 @@
       <c r="AT18" s="246"/>
       <c r="AU18" s="246"/>
       <c r="AV18" s="247">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AW18" s="247"/>
       <c r="AX18" s="247"/>
@@ -49356,7 +49368,7 @@
       <c r="AZ18" s="247"/>
       <c r="BA18" s="247"/>
       <c r="BB18" s="233">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BC18" s="233"/>
       <c r="BD18" s="233"/>
@@ -49396,7 +49408,7 @@
       <c r="J19" s="233"/>
       <c r="K19" s="233"/>
       <c r="L19" s="246" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M19" s="246"/>
       <c r="N19" s="246"/>
@@ -49434,7 +49446,7 @@
       <c r="AT19" s="246"/>
       <c r="AU19" s="246"/>
       <c r="AV19" s="247">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AW19" s="247"/>
       <c r="AX19" s="247"/>
@@ -49450,7 +49462,7 @@
       <c r="BF19" s="233"/>
       <c r="BG19" s="233"/>
       <c r="BH19" s="226">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BI19" s="227"/>
       <c r="BJ19" s="227"/>
@@ -49473,7 +49485,7 @@
       <c r="C20" s="225"/>
       <c r="D20" s="225"/>
       <c r="E20" s="233" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20" s="233"/>
       <c r="G20" s="233"/>
@@ -49482,7 +49494,7 @@
       <c r="J20" s="233"/>
       <c r="K20" s="233"/>
       <c r="L20" s="246" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M20" s="246"/>
       <c r="N20" s="246"/>
@@ -49520,7 +49532,7 @@
       <c r="AT20" s="246"/>
       <c r="AU20" s="246"/>
       <c r="AV20" s="247">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW20" s="247"/>
       <c r="AX20" s="247"/>
@@ -49528,7 +49540,7 @@
       <c r="AZ20" s="247"/>
       <c r="BA20" s="247"/>
       <c r="BB20" s="233">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="BC20" s="233"/>
       <c r="BD20" s="233"/>
@@ -49536,7 +49548,7 @@
       <c r="BF20" s="233"/>
       <c r="BG20" s="233"/>
       <c r="BH20" s="226">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BI20" s="227"/>
       <c r="BJ20" s="227"/>
@@ -49606,7 +49618,7 @@
       <c r="AT21" s="246"/>
       <c r="AU21" s="246"/>
       <c r="AV21" s="247">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AW21" s="247"/>
       <c r="AX21" s="247"/>
@@ -49614,7 +49626,7 @@
       <c r="AZ21" s="247"/>
       <c r="BA21" s="247"/>
       <c r="BB21" s="233">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="BC21" s="233"/>
       <c r="BD21" s="233"/>
@@ -49622,7 +49634,7 @@
       <c r="BF21" s="233"/>
       <c r="BG21" s="233"/>
       <c r="BH21" s="226">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BI21" s="227"/>
       <c r="BJ21" s="227"/>
@@ -49654,7 +49666,7 @@
       <c r="J22" s="233"/>
       <c r="K22" s="233"/>
       <c r="L22" s="246" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="M22" s="246"/>
       <c r="N22" s="246"/>
@@ -49692,7 +49704,7 @@
       <c r="AT22" s="246"/>
       <c r="AU22" s="246"/>
       <c r="AV22" s="247">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="AW22" s="247"/>
       <c r="AX22" s="247"/>
@@ -49700,7 +49712,7 @@
       <c r="AZ22" s="247"/>
       <c r="BA22" s="247"/>
       <c r="BB22" s="233">
-        <v>4.8999999999999995</v>
+        <v>4</v>
       </c>
       <c r="BC22" s="233"/>
       <c r="BD22" s="233"/>
@@ -49708,14 +49720,14 @@
       <c r="BF22" s="233"/>
       <c r="BG22" s="233"/>
       <c r="BH22" s="226">
-        <v>-8.881784197001252e-16</v>
+        <v>4</v>
       </c>
       <c r="BI22" s="227"/>
       <c r="BJ22" s="227"/>
       <c r="BK22" s="227"/>
       <c r="BL22" s="228"/>
       <c r="BM22" s="226" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="BN22" s="227"/>
       <c r="BO22" s="227"/>
@@ -49731,7 +49743,7 @@
       <c r="C23" s="225"/>
       <c r="D23" s="225"/>
       <c r="E23" s="233" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" s="233"/>
       <c r="G23" s="233"/>
@@ -49740,7 +49752,7 @@
       <c r="J23" s="233"/>
       <c r="K23" s="233"/>
       <c r="L23" s="246" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M23" s="246"/>
       <c r="N23" s="246"/>
@@ -49778,7 +49790,7 @@
       <c r="AT23" s="246"/>
       <c r="AU23" s="246"/>
       <c r="AV23" s="247">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW23" s="247"/>
       <c r="AX23" s="247"/>
@@ -49786,7 +49798,7 @@
       <c r="AZ23" s="247"/>
       <c r="BA23" s="247"/>
       <c r="BB23" s="233">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="BC23" s="233"/>
       <c r="BD23" s="233"/>
@@ -49794,14 +49806,14 @@
       <c r="BF23" s="233"/>
       <c r="BG23" s="233"/>
       <c r="BH23" s="226">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="BI23" s="227"/>
       <c r="BJ23" s="227"/>
       <c r="BK23" s="227"/>
       <c r="BL23" s="228"/>
       <c r="BM23" s="226" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="BN23" s="227"/>
       <c r="BO23" s="227"/>
@@ -49826,7 +49838,7 @@
       <c r="J24" s="233"/>
       <c r="K24" s="233"/>
       <c r="L24" s="246" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M24" s="246"/>
       <c r="N24" s="246"/>
@@ -49864,7 +49876,7 @@
       <c r="AT24" s="246"/>
       <c r="AU24" s="246"/>
       <c r="AV24" s="247">
-        <v>1.6</v>
+        <v>4.9</v>
       </c>
       <c r="AW24" s="247"/>
       <c r="AX24" s="247"/>
@@ -49872,7 +49884,7 @@
       <c r="AZ24" s="247"/>
       <c r="BA24" s="247"/>
       <c r="BB24" s="233">
-        <v>2.2</v>
+        <v>4.8999999999999995</v>
       </c>
       <c r="BC24" s="233"/>
       <c r="BD24" s="233"/>
@@ -49880,7 +49892,7 @@
       <c r="BF24" s="233"/>
       <c r="BG24" s="233"/>
       <c r="BH24" s="226">
-        <v>0.6000000000000001</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="BI24" s="227"/>
       <c r="BJ24" s="227"/>
@@ -49903,7 +49915,7 @@
       <c r="C25" s="233"/>
       <c r="D25" s="233"/>
       <c r="E25" s="233" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F25" s="233"/>
       <c r="G25" s="233"/>
@@ -49912,7 +49924,7 @@
       <c r="J25" s="233"/>
       <c r="K25" s="233"/>
       <c r="L25" s="248" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="M25" s="248"/>
       <c r="N25" s="248"/>
@@ -49950,7 +49962,7 @@
       <c r="AT25" s="248"/>
       <c r="AU25" s="248"/>
       <c r="AV25" s="247">
-        <v>16</v>
+        <v>1.6</v>
       </c>
       <c r="AW25" s="247"/>
       <c r="AX25" s="247"/>
@@ -49958,7 +49970,7 @@
       <c r="AZ25" s="247"/>
       <c r="BA25" s="247"/>
       <c r="BB25" s="233">
-        <v>24</v>
+        <v>2.2</v>
       </c>
       <c r="BC25" s="233"/>
       <c r="BD25" s="233"/>
@@ -49966,7 +49978,7 @@
       <c r="BF25" s="233"/>
       <c r="BG25" s="233"/>
       <c r="BH25" s="226">
-        <v>8</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="BI25" s="227"/>
       <c r="BJ25" s="227"/>
@@ -49989,7 +50001,7 @@
       <c r="C26" s="233"/>
       <c r="D26" s="233"/>
       <c r="E26" s="233" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F26" s="233"/>
       <c r="G26" s="233"/>
@@ -49998,7 +50010,7 @@
       <c r="J26" s="233"/>
       <c r="K26" s="233"/>
       <c r="L26" s="248" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M26" s="248"/>
       <c r="N26" s="248"/>
@@ -50044,7 +50056,7 @@
       <c r="AZ26" s="247"/>
       <c r="BA26" s="247"/>
       <c r="BB26" s="233">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BC26" s="233"/>
       <c r="BD26" s="233"/>
@@ -50052,7 +50064,7 @@
       <c r="BF26" s="233"/>
       <c r="BG26" s="233"/>
       <c r="BH26" s="226">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BI26" s="227"/>
       <c r="BJ26" s="227"/>
@@ -50075,7 +50087,7 @@
       <c r="C27" s="233"/>
       <c r="D27" s="233"/>
       <c r="E27" s="233" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F27" s="233"/>
       <c r="G27" s="233"/>
@@ -50084,7 +50096,7 @@
       <c r="J27" s="233"/>
       <c r="K27" s="233"/>
       <c r="L27" s="248" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="M27" s="248"/>
       <c r="N27" s="248"/>
@@ -50122,7 +50134,7 @@
       <c r="AT27" s="248"/>
       <c r="AU27" s="248"/>
       <c r="AV27" s="247">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="AW27" s="247"/>
       <c r="AX27" s="247"/>
@@ -50130,7 +50142,7 @@
       <c r="AZ27" s="247"/>
       <c r="BA27" s="247"/>
       <c r="BB27" s="233">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="BC27" s="233"/>
       <c r="BD27" s="233"/>
@@ -50138,7 +50150,7 @@
       <c r="BF27" s="233"/>
       <c r="BG27" s="233"/>
       <c r="BH27" s="226">
-        <v>-4</v>
+        <v>8</v>
       </c>
       <c r="BI27" s="227"/>
       <c r="BJ27" s="227"/>
@@ -50161,7 +50173,7 @@
       <c r="C28" s="233"/>
       <c r="D28" s="233"/>
       <c r="E28" s="226" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F28" s="227"/>
       <c r="G28" s="227"/>
@@ -50170,7 +50182,7 @@
       <c r="J28" s="227"/>
       <c r="K28" s="228"/>
       <c r="L28" s="229" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M28" s="249"/>
       <c r="N28" s="249"/>
@@ -50208,7 +50220,7 @@
       <c r="AT28" s="249"/>
       <c r="AU28" s="250"/>
       <c r="AV28" s="251">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AW28" s="252"/>
       <c r="AX28" s="252"/>
@@ -50216,7 +50228,7 @@
       <c r="AZ28" s="252"/>
       <c r="BA28" s="253"/>
       <c r="BB28" s="226">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BC28" s="227"/>
       <c r="BD28" s="227"/>
@@ -50224,7 +50236,7 @@
       <c r="BF28" s="227"/>
       <c r="BG28" s="228"/>
       <c r="BH28" s="226">
-        <v>-6</v>
+        <v>3</v>
       </c>
       <c r="BI28" s="227"/>
       <c r="BJ28" s="227"/>
@@ -50240,18 +50252,24 @@
       <c r="BR28" s="241"/>
     </row>
     <row r="29" ht="19.95" customHeight="1" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A29" s="245"/>
+      <c r="A29" s="245">
+        <v>23</v>
+      </c>
       <c r="B29" s="233"/>
       <c r="C29" s="233"/>
       <c r="D29" s="233"/>
-      <c r="E29" s="226"/>
+      <c r="E29" s="226" t="s">
+        <v>91</v>
+      </c>
       <c r="F29" s="227"/>
       <c r="G29" s="227"/>
       <c r="H29" s="227"/>
       <c r="I29" s="227"/>
       <c r="J29" s="227"/>
       <c r="K29" s="228"/>
-      <c r="L29" s="229"/>
+      <c r="L29" s="229" t="s">
+        <v>81</v>
+      </c>
       <c r="M29" s="249"/>
       <c r="N29" s="249"/>
       <c r="O29" s="249"/>
@@ -50287,24 +50305,32 @@
       <c r="AS29" s="249"/>
       <c r="AT29" s="249"/>
       <c r="AU29" s="250"/>
-      <c r="AV29" s="251"/>
+      <c r="AV29" s="251">
+        <v>4</v>
+      </c>
       <c r="AW29" s="252"/>
       <c r="AX29" s="252"/>
       <c r="AY29" s="252"/>
       <c r="AZ29" s="252"/>
       <c r="BA29" s="253"/>
-      <c r="BB29" s="226"/>
+      <c r="BB29" s="226">
+        <v>0</v>
+      </c>
       <c r="BC29" s="227"/>
       <c r="BD29" s="227"/>
       <c r="BE29" s="227"/>
       <c r="BF29" s="227"/>
       <c r="BG29" s="228"/>
-      <c r="BH29" s="226"/>
+      <c r="BH29" s="226">
+        <v>-4</v>
+      </c>
       <c r="BI29" s="227"/>
       <c r="BJ29" s="227"/>
       <c r="BK29" s="227"/>
       <c r="BL29" s="228"/>
-      <c r="BM29" s="226"/>
+      <c r="BM29" s="226" t="s">
+        <v>57</v>
+      </c>
       <c r="BN29" s="227"/>
       <c r="BO29" s="227"/>
       <c r="BP29" s="227"/>
@@ -50312,18 +50338,24 @@
       <c r="BR29" s="241"/>
     </row>
     <row r="30" ht="19.95" customHeight="1" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A30" s="224"/>
+      <c r="A30" s="224">
+        <v>24</v>
+      </c>
       <c r="B30" s="225"/>
       <c r="C30" s="225"/>
       <c r="D30" s="225"/>
-      <c r="E30" s="233"/>
+      <c r="E30" s="233" t="s">
+        <v>92</v>
+      </c>
       <c r="F30" s="233"/>
       <c r="G30" s="233"/>
       <c r="H30" s="233"/>
       <c r="I30" s="233"/>
       <c r="J30" s="233"/>
       <c r="K30" s="233"/>
-      <c r="L30" s="248"/>
+      <c r="L30" s="248" t="s">
+        <v>81</v>
+      </c>
       <c r="M30" s="248"/>
       <c r="N30" s="248"/>
       <c r="O30" s="248"/>
@@ -50359,24 +50391,32 @@
       <c r="AS30" s="248"/>
       <c r="AT30" s="248"/>
       <c r="AU30" s="248"/>
-      <c r="AV30" s="251"/>
+      <c r="AV30" s="251">
+        <v>6</v>
+      </c>
       <c r="AW30" s="252"/>
       <c r="AX30" s="252"/>
       <c r="AY30" s="252"/>
       <c r="AZ30" s="252"/>
       <c r="BA30" s="253"/>
-      <c r="BB30" s="226"/>
+      <c r="BB30" s="226">
+        <v>0</v>
+      </c>
       <c r="BC30" s="227"/>
       <c r="BD30" s="227"/>
       <c r="BE30" s="227"/>
       <c r="BF30" s="227"/>
       <c r="BG30" s="228"/>
-      <c r="BH30" s="226"/>
+      <c r="BH30" s="226">
+        <v>-6</v>
+      </c>
       <c r="BI30" s="227"/>
       <c r="BJ30" s="227"/>
       <c r="BK30" s="227"/>
       <c r="BL30" s="228"/>
-      <c r="BM30" s="226"/>
+      <c r="BM30" s="226" t="s">
+        <v>57</v>
+      </c>
       <c r="BN30" s="227"/>
       <c r="BO30" s="227"/>
       <c r="BP30" s="227"/>
@@ -50384,18 +50424,24 @@
       <c r="BR30" s="241"/>
     </row>
     <row r="31" ht="19.95" customHeight="1" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A31" s="224"/>
+      <c r="A31" s="224">
+        <v>25</v>
+      </c>
       <c r="B31" s="225"/>
       <c r="C31" s="225"/>
       <c r="D31" s="225"/>
-      <c r="E31" s="233"/>
+      <c r="E31" s="233" t="s">
+        <v>93</v>
+      </c>
       <c r="F31" s="233"/>
       <c r="G31" s="233"/>
       <c r="H31" s="233"/>
       <c r="I31" s="233"/>
       <c r="J31" s="233"/>
       <c r="K31" s="233"/>
-      <c r="L31" s="248"/>
+      <c r="L31" s="248" t="s">
+        <v>86</v>
+      </c>
       <c r="M31" s="248"/>
       <c r="N31" s="248"/>
       <c r="O31" s="248"/>
@@ -50431,24 +50477,32 @@
       <c r="AS31" s="248"/>
       <c r="AT31" s="248"/>
       <c r="AU31" s="248"/>
-      <c r="AV31" s="251"/>
+      <c r="AV31" s="251">
+        <v>0</v>
+      </c>
       <c r="AW31" s="252"/>
       <c r="AX31" s="252"/>
       <c r="AY31" s="252"/>
       <c r="AZ31" s="252"/>
       <c r="BA31" s="253"/>
-      <c r="BB31" s="226"/>
+      <c r="BB31" s="226">
+        <v>0.6</v>
+      </c>
       <c r="BC31" s="227"/>
       <c r="BD31" s="227"/>
       <c r="BE31" s="227"/>
       <c r="BF31" s="227"/>
       <c r="BG31" s="228"/>
-      <c r="BH31" s="226"/>
+      <c r="BH31" s="226">
+        <v>0.6</v>
+      </c>
       <c r="BI31" s="227"/>
       <c r="BJ31" s="227"/>
       <c r="BK31" s="227"/>
       <c r="BL31" s="228"/>
-      <c r="BM31" s="226"/>
+      <c r="BM31" s="226" t="s">
+        <v>72</v>
+      </c>
       <c r="BN31" s="227"/>
       <c r="BO31" s="227"/>
       <c r="BP31" s="227"/>
@@ -51105,7 +51159,7 @@
     </row>
     <row r="41" ht="19.95" customHeight="1" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A41" s="255" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B41" s="256"/>
       <c r="C41" s="256"/>

</xml_diff>